<commit_message>
20250106 calculo de fuste mixto
</commit_message>
<xml_diff>
--- a/Data/datos_terreno_4.xlsx
+++ b/Data/datos_terreno_4.xlsx
@@ -41,10 +41,10 @@
     <t>Tipo Cálculo</t>
   </si>
   <si>
-    <t>Drenado</t>
-  </si>
-  <si>
-    <t>No drenado</t>
+    <t>d</t>
+  </si>
+  <si>
+    <t>nd</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
         <v>20</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>